<commit_message>
beautiful soup python assignment
</commit_message>
<xml_diff>
--- a/classes/BSinCS.xlsx
+++ b/classes/BSinCS.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Add Classes" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Classes!$A$1:$H$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Classes!$A$1:$H$89</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="391">
   <si>
     <t>Alias</t>
   </si>
@@ -1195,13 +1195,16 @@
   </si>
   <si>
     <t>UOFM</t>
+  </si>
+  <si>
+    <t>Internet History, Technology, and Security</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1257,6 +1260,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1427,11 +1438,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1503,8 +1515,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1512,17 +1525,21 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2023,13 +2040,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2070,16 +2087,16 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="46"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="15"/>
@@ -2349,260 +2366,254 @@
         <v>388</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>42</v>
-      </c>
+    <row r="15" spans="1:8" ht="15" customHeight="1">
+      <c r="A15" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="B15" s="43" t="s">
+        <v>389</v>
+      </c>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43" t="s">
+        <v>386</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>390</v>
+      </c>
+      <c r="G15" s="43"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="15"/>
-      <c r="B16" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19" t="s">
+      <c r="B16" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>45</v>
+      <c r="F16" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="15"/>
-      <c r="B17" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>50</v>
+      <c r="B17" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="15"/>
       <c r="B18" s="16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>47</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="15"/>
       <c r="B19" s="16" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="15"/>
       <c r="B20" s="16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>57</v>
       </c>
       <c r="E20" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="15"/>
+      <c r="B21" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F21" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G21" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H21" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="43" t="s">
+    <row r="22" spans="1:8">
+      <c r="A22" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="45"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="15"/>
-      <c r="B22" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="26" t="s">
-        <v>69</v>
-      </c>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="46"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="15"/>
       <c r="B23" s="24" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>57</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="H23" s="26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="15"/>
       <c r="B24" s="24" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="H24" s="26" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="15"/>
       <c r="B25" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C25" s="24" t="s">
         <v>67</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="H25" s="26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="25">
       <c r="A26" s="15"/>
       <c r="B26" s="24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C26" s="24" t="s">
         <v>67</v>
@@ -2611,560 +2622,564 @@
         <v>10</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G26" s="24" t="s">
         <v>41</v>
       </c>
       <c r="H26" s="26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="15"/>
       <c r="B27" s="24" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C27" s="24" t="s">
         <v>67</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G27" s="24" t="s">
         <v>41</v>
       </c>
       <c r="H27" s="26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="15"/>
+      <c r="B28" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" s="26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="43" t="s">
+    <row r="29" spans="1:8">
+      <c r="A29" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="45"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="15"/>
-      <c r="B29" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="F29" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="G29" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="26" t="s">
-        <v>94</v>
-      </c>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="46"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="15"/>
       <c r="B30" s="24" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D30" s="24" t="s">
         <v>21</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G30" s="24" t="s">
         <v>13</v>
       </c>
       <c r="H30" s="26" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="15"/>
       <c r="B31" s="24" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="H31" s="26" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="15"/>
       <c r="B32" s="24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C32" s="24" t="s">
         <v>67</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="H32" s="26" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="15"/>
-      <c r="B33" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="27" t="s">
+      <c r="B33" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="F33" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="G33" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="H33" s="29" t="s">
-        <v>111</v>
+      <c r="E33" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="26" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="15"/>
-      <c r="B34" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="E34" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="F34" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="G34" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="H34" s="26" t="s">
-        <v>115</v>
+      <c r="B34" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G34" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="15"/>
       <c r="B35" s="24" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D35" s="24" t="s">
         <v>113</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F35" s="25" t="s">
         <v>113</v>
       </c>
       <c r="G35" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="15"/>
+      <c r="B36" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="H35" s="26" t="s">
+      <c r="D36" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="H36" s="26" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="43" t="s">
+    <row r="37" spans="1:8">
+      <c r="A37" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="45"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="15"/>
-      <c r="B37" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="E37" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="F37" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="G37" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" s="26" t="s">
-        <v>124</v>
-      </c>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="46"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="15"/>
       <c r="B38" s="24" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D38" s="24" t="s">
         <v>121</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="H38" s="26" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="15"/>
       <c r="B39" s="24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="H39" s="26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="15"/>
       <c r="B40" s="24" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D40" s="24" t="s">
         <v>129</v>
       </c>
       <c r="E40" s="24" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="H40" s="26" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="15"/>
-      <c r="B41" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="F41" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="G41" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="29" t="s">
-        <v>140</v>
+      <c r="B41" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="E41" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="F41" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G41" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="H41" s="26" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="15"/>
-      <c r="B42" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="F42" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="G42" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="26" t="s">
-        <v>145</v>
+      <c r="B42" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="F42" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="G42" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="29" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="15"/>
       <c r="B43" s="24" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D43" s="24" t="s">
         <v>142</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G43" s="24" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="H43" s="26" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="15"/>
       <c r="B44" s="24" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="H44" s="26" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="15"/>
       <c r="B45" s="24" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C45" s="24" t="s">
         <v>67</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E45" s="24" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G45" s="24" t="s">
         <v>41</v>
       </c>
       <c r="H45" s="26" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="15"/>
       <c r="B46" s="24" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D46" s="24" t="s">
         <v>156</v>
       </c>
       <c r="E46" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="F46" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="G46" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="H46" s="26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="15"/>
+      <c r="B47" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="E47" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="F46" s="25" t="s">
+      <c r="F47" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="G46" s="42" t="s">
+      <c r="G47" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="H46" s="32" t="s">
+      <c r="H47" s="32" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="43" t="s">
+    <row r="48" spans="1:8">
+      <c r="A48" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="B47" s="44"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="34"/>
-    </row>
-    <row r="48" spans="1:8" ht="39">
-      <c r="A48" s="15"/>
-      <c r="B48" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D48" s="30" t="s">
-        <v>166</v>
-      </c>
-      <c r="E48" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="F48" s="38" t="s">
-        <v>168</v>
-      </c>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="34"/>
+    </row>
+    <row r="49" spans="1:8" ht="39">
       <c r="A49" s="15"/>
       <c r="B49" s="30" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C49" s="30" t="s">
         <v>47</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>114</v>
+        <v>166</v>
       </c>
       <c r="E49" s="30" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F49" s="38" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="52">
+    <row r="50" spans="1:8">
       <c r="A50" s="15"/>
-      <c r="B50" s="31" t="s">
-        <v>172</v>
-      </c>
-      <c r="C50" s="31" t="s">
-        <v>173</v>
-      </c>
-      <c r="D50" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="E50" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="F50" s="39" t="s">
-        <v>176</v>
+      <c r="B50" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="F50" s="38" t="s">
+        <v>171</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" ht="26">
+    <row r="51" spans="1:8" ht="52">
       <c r="A51" s="15"/>
       <c r="B51" s="31" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C51" s="31" t="s">
         <v>173</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E51" s="31" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F51" s="39" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -3172,203 +3187,203 @@
     <row r="52" spans="1:8" ht="26">
       <c r="A52" s="15"/>
       <c r="B52" s="31" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>21</v>
+        <v>173</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E52" s="31" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F52" s="39" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="39">
+    <row r="53" spans="1:8" ht="26">
       <c r="A53" s="15"/>
       <c r="B53" s="31" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C53" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E53" s="31" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F53" s="39" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="26">
+    <row r="54" spans="1:8" ht="39">
       <c r="A54" s="15"/>
-      <c r="B54" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="C54" s="30" t="s">
+      <c r="B54" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D54" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="E54" s="30" t="s">
-        <v>191</v>
-      </c>
-      <c r="F54" s="38" t="s">
-        <v>192</v>
+      <c r="D54" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="E54" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="F54" s="39" t="s">
+        <v>188</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" ht="26">
       <c r="A55" s="15"/>
       <c r="B55" s="30" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C55" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D55" s="30" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E55" s="30" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F55" s="38" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="26">
+    <row r="56" spans="1:8">
       <c r="A56" s="15"/>
       <c r="B56" s="30" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C56" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>130</v>
+        <v>194</v>
       </c>
       <c r="E56" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F56" s="38" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="45" customHeight="1">
+    <row r="57" spans="1:8" ht="26">
       <c r="A57" s="15"/>
-      <c r="B57" s="47" t="s">
+      <c r="B57" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="C57" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="E57" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="F57" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:8" ht="45" customHeight="1">
+      <c r="A58" s="15"/>
+      <c r="B58" s="51" t="s">
         <v>200</v>
       </c>
-      <c r="C57" s="47" t="s">
+      <c r="C58" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="D57" s="47" t="s">
+      <c r="D58" s="51" t="s">
         <v>201</v>
       </c>
-      <c r="E57" s="47" t="s">
+      <c r="E58" s="51" t="s">
         <v>202</v>
       </c>
-      <c r="F57" s="38" t="s">
+      <c r="F58" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="G57" s="46"/>
-      <c r="H57" s="46"/>
-    </row>
-    <row r="58" spans="1:8" ht="30" customHeight="1">
-      <c r="A58" s="15"/>
-      <c r="B58" s="47"/>
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="38" t="s">
+      <c r="G58" s="50"/>
+      <c r="H58" s="50"/>
+    </row>
+    <row r="59" spans="1:8" ht="30" customHeight="1">
+      <c r="A59" s="15"/>
+      <c r="B59" s="51"/>
+      <c r="C59" s="51"/>
+      <c r="D59" s="51"/>
+      <c r="E59" s="51"/>
+      <c r="F59" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="G58" s="46"/>
-      <c r="H58" s="46"/>
-    </row>
-    <row r="59" spans="1:8" ht="45" customHeight="1">
-      <c r="A59" s="15"/>
-      <c r="B59" s="47" t="s">
+      <c r="G59" s="50"/>
+      <c r="H59" s="50"/>
+    </row>
+    <row r="60" spans="1:8" ht="45" customHeight="1">
+      <c r="A60" s="15"/>
+      <c r="B60" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="C59" s="47" t="s">
+      <c r="C60" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="D59" s="47" t="s">
+      <c r="D60" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="E59" s="47" t="s">
+      <c r="E60" s="51" t="s">
         <v>207</v>
       </c>
-      <c r="F59" s="38" t="s">
+      <c r="F60" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="G59" s="46"/>
-      <c r="H59" s="46"/>
-    </row>
-    <row r="60" spans="1:8" ht="15" customHeight="1">
-      <c r="A60" s="15"/>
-      <c r="B60" s="47"/>
-      <c r="C60" s="47"/>
-      <c r="D60" s="47"/>
-      <c r="E60" s="47"/>
-      <c r="F60" s="38" t="s">
+      <c r="G60" s="50"/>
+      <c r="H60" s="50"/>
+    </row>
+    <row r="61" spans="1:8" ht="15" customHeight="1">
+      <c r="A61" s="15"/>
+      <c r="B61" s="51"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="51"/>
+      <c r="E61" s="51"/>
+      <c r="F61" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="G60" s="46"/>
-      <c r="H60" s="46"/>
-    </row>
-    <row r="61" spans="1:8" ht="39">
-      <c r="A61" s="15"/>
-      <c r="B61" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="C61" s="31" t="s">
-        <v>211</v>
-      </c>
-      <c r="D61" s="31" t="s">
-        <v>212</v>
-      </c>
-      <c r="E61" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="F61" s="39" t="s">
-        <v>214</v>
-      </c>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-    </row>
-    <row r="62" spans="1:8" ht="26">
+      <c r="G61" s="50"/>
+      <c r="H61" s="50"/>
+    </row>
+    <row r="62" spans="1:8" ht="39">
       <c r="A62" s="15"/>
       <c r="B62" s="31" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C62" s="31" t="s">
         <v>211</v>
       </c>
       <c r="D62" s="31" t="s">
-        <v>96</v>
+        <v>212</v>
       </c>
       <c r="E62" s="31" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F62" s="39" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -3376,7 +3391,7 @@
     <row r="63" spans="1:8" ht="26">
       <c r="A63" s="15"/>
       <c r="B63" s="31" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C63" s="31" t="s">
         <v>211</v>
@@ -3385,50 +3400,50 @@
         <v>96</v>
       </c>
       <c r="E63" s="31" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F63" s="39" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" ht="26">
       <c r="A64" s="15"/>
       <c r="B64" s="31" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C64" s="31" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="D64" s="31" t="s">
-        <v>223</v>
+        <v>96</v>
       </c>
       <c r="E64" s="31" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F64" s="39" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="26">
+    <row r="65" spans="1:8">
       <c r="A65" s="15"/>
       <c r="B65" s="31" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D65" s="31" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E65" s="31" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F65" s="39" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
@@ -3436,59 +3451,59 @@
     <row r="66" spans="1:8" ht="26">
       <c r="A66" s="15"/>
       <c r="B66" s="31" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C66" s="31" t="s">
         <v>227</v>
       </c>
       <c r="D66" s="31" t="s">
-        <v>11</v>
+        <v>228</v>
       </c>
       <c r="E66" s="31" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F66" s="39" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" ht="26">
       <c r="A67" s="15"/>
       <c r="B67" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C67" s="31" t="s">
         <v>227</v>
       </c>
       <c r="D67" s="31" t="s">
-        <v>235</v>
+        <v>11</v>
       </c>
       <c r="E67" s="31" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F67" s="39" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="26">
+    <row r="68" spans="1:8">
       <c r="A68" s="15"/>
       <c r="B68" s="31" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E68" s="31" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F68" s="39" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
@@ -3496,179 +3511,179 @@
     <row r="69" spans="1:8" ht="26">
       <c r="A69" s="15"/>
       <c r="B69" s="31" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C69" s="31" t="s">
         <v>239</v>
       </c>
       <c r="D69" s="31" t="s">
-        <v>178</v>
+        <v>240</v>
       </c>
       <c r="E69" s="31" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F69" s="39" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" ht="26">
       <c r="A70" s="15"/>
-      <c r="B70" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="C70" s="30" t="s">
+      <c r="B70" s="31" t="s">
+        <v>243</v>
+      </c>
+      <c r="C70" s="31" t="s">
         <v>239</v>
       </c>
-      <c r="D70" s="30" t="s">
+      <c r="D70" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="E70" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="F70" s="38" t="s">
-        <v>248</v>
+      <c r="E70" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="F70" s="39" t="s">
+        <v>245</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="52">
+    <row r="71" spans="1:8">
       <c r="A71" s="15"/>
-      <c r="B71" s="31" t="s">
-        <v>249</v>
-      </c>
-      <c r="C71" s="31" t="s">
-        <v>250</v>
-      </c>
-      <c r="D71" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="E71" s="31" t="s">
-        <v>252</v>
-      </c>
-      <c r="F71" s="39" t="s">
-        <v>253</v>
+      <c r="B71" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="C71" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="D71" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="F71" s="38" t="s">
+        <v>248</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" ht="52">
       <c r="A72" s="15"/>
       <c r="B72" s="31" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C72" s="31" t="s">
         <v>250</v>
       </c>
       <c r="D72" s="31" t="s">
-        <v>130</v>
+        <v>251</v>
       </c>
       <c r="E72" s="31" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F72" s="39" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="15"/>
-      <c r="B73" s="30" t="s">
-        <v>257</v>
-      </c>
-      <c r="C73" s="30" t="s">
+      <c r="B73" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="C73" s="31" t="s">
         <v>250</v>
       </c>
-      <c r="D73" s="30" t="s">
+      <c r="D73" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="E73" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="F73" s="38" t="s">
-        <v>259</v>
+      <c r="E73" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="F73" s="39" t="s">
+        <v>256</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="26">
+    <row r="74" spans="1:8">
       <c r="A74" s="15"/>
-      <c r="B74" s="31" t="s">
-        <v>260</v>
-      </c>
-      <c r="C74" s="31" t="s">
-        <v>261</v>
-      </c>
-      <c r="D74" s="31" t="s">
-        <v>262</v>
-      </c>
-      <c r="E74" s="31" t="s">
-        <v>263</v>
-      </c>
-      <c r="F74" s="39" t="s">
-        <v>264</v>
+      <c r="B74" s="30" t="s">
+        <v>257</v>
+      </c>
+      <c r="C74" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="D74" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="E74" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="F74" s="38" t="s">
+        <v>259</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="39">
+    <row r="75" spans="1:8" ht="26">
       <c r="A75" s="15"/>
-      <c r="B75" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="C75" s="30" t="s">
+      <c r="B75" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="C75" s="31" t="s">
         <v>261</v>
       </c>
-      <c r="D75" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="E75" s="30" t="s">
+      <c r="D75" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="E75" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="F75" s="38" t="s">
-        <v>266</v>
+      <c r="F75" s="39" t="s">
+        <v>264</v>
       </c>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" ht="39">
       <c r="A76" s="15"/>
-      <c r="B76" s="31" t="s">
-        <v>267</v>
-      </c>
-      <c r="C76" s="31" t="s">
+      <c r="B76" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="C76" s="30" t="s">
         <v>261</v>
       </c>
-      <c r="D76" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="E76" s="31" t="s">
-        <v>268</v>
-      </c>
-      <c r="F76" s="39" t="s">
-        <v>269</v>
+      <c r="D76" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>263</v>
+      </c>
+      <c r="F76" s="38" t="s">
+        <v>266</v>
       </c>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="15"/>
-      <c r="B77" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="C77" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="D77" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="E77" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="F77" s="38" t="s">
-        <v>273</v>
+      <c r="B77" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="C77" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="D77" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="E77" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="F77" s="39" t="s">
+        <v>269</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
@@ -3676,59 +3691,59 @@
     <row r="78" spans="1:8">
       <c r="A78" s="15"/>
       <c r="B78" s="30" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C78" s="30" t="s">
         <v>271</v>
       </c>
       <c r="D78" s="30" t="s">
-        <v>130</v>
+        <v>272</v>
       </c>
       <c r="E78" s="30" t="s">
         <v>271</v>
       </c>
       <c r="F78" s="38" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" ht="39">
+    <row r="79" spans="1:8">
       <c r="A79" s="15"/>
       <c r="B79" s="30" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C79" s="30" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D79" s="30" t="s">
-        <v>278</v>
+        <v>130</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="F79" s="38" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" ht="26">
+    <row r="80" spans="1:8" ht="39">
       <c r="A80" s="15"/>
       <c r="B80" s="30" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C80" s="30" t="s">
         <v>277</v>
       </c>
       <c r="D80" s="30" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F80" s="38" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -3736,198 +3751,218 @@
     <row r="81" spans="1:8" ht="26">
       <c r="A81" s="15"/>
       <c r="B81" s="30" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C81" s="30" t="s">
         <v>277</v>
       </c>
       <c r="D81" s="30" t="s">
-        <v>96</v>
+        <v>282</v>
       </c>
       <c r="E81" s="30" t="s">
         <v>283</v>
       </c>
       <c r="F81" s="38" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" ht="39">
+    <row r="82" spans="1:8" ht="26">
       <c r="A82" s="15"/>
-      <c r="B82" s="31" t="s">
-        <v>287</v>
-      </c>
-      <c r="C82" s="31" t="s">
-        <v>288</v>
-      </c>
-      <c r="D82" s="31" t="s">
-        <v>289</v>
-      </c>
-      <c r="E82" s="31" t="s">
-        <v>290</v>
-      </c>
-      <c r="F82" s="39" t="s">
-        <v>291</v>
+      <c r="B82" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="C82" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="D82" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="F82" s="38" t="s">
+        <v>286</v>
       </c>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="26">
+    <row r="83" spans="1:8" ht="39">
       <c r="A83" s="15"/>
-      <c r="B83" s="30" t="s">
-        <v>292</v>
-      </c>
-      <c r="C83" s="30" t="s">
+      <c r="B83" s="31" t="s">
+        <v>287</v>
+      </c>
+      <c r="C83" s="31" t="s">
         <v>288</v>
       </c>
-      <c r="D83" s="30" t="s">
-        <v>293</v>
-      </c>
-      <c r="E83" s="30" t="s">
-        <v>294</v>
-      </c>
-      <c r="F83" s="38" t="s">
-        <v>295</v>
+      <c r="D83" s="31" t="s">
+        <v>289</v>
+      </c>
+      <c r="E83" s="31" t="s">
+        <v>290</v>
+      </c>
+      <c r="F83" s="39" t="s">
+        <v>291</v>
       </c>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" ht="26">
       <c r="A84" s="15"/>
-      <c r="B84" s="31" t="s">
-        <v>296</v>
-      </c>
-      <c r="C84" s="31" t="s">
+      <c r="B84" s="30" t="s">
+        <v>292</v>
+      </c>
+      <c r="C84" s="30" t="s">
         <v>288</v>
       </c>
-      <c r="D84" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="E84" s="31" t="s">
-        <v>297</v>
-      </c>
-      <c r="F84" s="39" t="s">
-        <v>298</v>
+      <c r="D84" s="30" t="s">
+        <v>293</v>
+      </c>
+      <c r="E84" s="30" t="s">
+        <v>294</v>
+      </c>
+      <c r="F84" s="38" t="s">
+        <v>295</v>
       </c>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" ht="39">
+    <row r="85" spans="1:8">
       <c r="A85" s="15"/>
       <c r="B85" s="31" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C85" s="31" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="D85" s="31" t="s">
-        <v>301</v>
+        <v>114</v>
       </c>
       <c r="E85" s="31" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F85" s="39" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="52">
+    <row r="86" spans="1:8" ht="39">
       <c r="A86" s="15"/>
       <c r="B86" s="31" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C86" s="31" t="s">
         <v>300</v>
       </c>
       <c r="D86" s="31" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E86" s="31" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="F86" s="39" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" ht="26">
+    <row r="87" spans="1:8" ht="52">
       <c r="A87" s="15"/>
-      <c r="B87" s="30" t="s">
-        <v>308</v>
-      </c>
-      <c r="C87" s="30" t="s">
+      <c r="B87" s="31" t="s">
+        <v>304</v>
+      </c>
+      <c r="C87" s="31" t="s">
         <v>300</v>
       </c>
-      <c r="D87" s="30" t="s">
-        <v>309</v>
-      </c>
-      <c r="E87" s="30" t="s">
-        <v>310</v>
-      </c>
-      <c r="F87" s="38" t="s">
-        <v>311</v>
+      <c r="D87" s="31" t="s">
+        <v>305</v>
+      </c>
+      <c r="E87" s="31" t="s">
+        <v>306</v>
+      </c>
+      <c r="F87" s="39" t="s">
+        <v>307</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
     <row r="88" spans="1:8" ht="26">
       <c r="A88" s="15"/>
-      <c r="B88" s="31" t="s">
-        <v>312</v>
-      </c>
-      <c r="C88" s="31" t="s">
+      <c r="B88" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="C88" s="30" t="s">
         <v>300</v>
       </c>
-      <c r="D88" s="31" t="s">
-        <v>313</v>
-      </c>
-      <c r="E88" s="31" t="s">
-        <v>314</v>
-      </c>
-      <c r="F88" s="39" t="s">
-        <v>315</v>
+      <c r="D88" s="30" t="s">
+        <v>309</v>
+      </c>
+      <c r="E88" s="30" t="s">
+        <v>310</v>
+      </c>
+      <c r="F88" s="38" t="s">
+        <v>311</v>
       </c>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="4"/>
+    <row r="89" spans="1:8" ht="26">
+      <c r="A89" s="15"/>
+      <c r="B89" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="C89" s="31" t="s">
+        <v>300</v>
+      </c>
+      <c r="D89" s="31" t="s">
+        <v>313</v>
+      </c>
+      <c r="E89" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="F89" s="39" t="s">
+        <v>315</v>
+      </c>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
+    <row r="90" spans="1:8">
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H88"/>
+  <autoFilter ref="A1:H89"/>
   <mergeCells count="23">
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="H60:H61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1"/>
@@ -3937,76 +3972,76 @@
     <hyperlink ref="H10" r:id="rId5"/>
     <hyperlink ref="H12" r:id="rId6"/>
     <hyperlink ref="H13" r:id="rId7"/>
-    <hyperlink ref="H15" r:id="rId8"/>
-    <hyperlink ref="H16" r:id="rId9"/>
-    <hyperlink ref="H17" r:id="rId10"/>
-    <hyperlink ref="H18" r:id="rId11"/>
-    <hyperlink ref="H19" r:id="rId12"/>
-    <hyperlink ref="H20" r:id="rId13"/>
-    <hyperlink ref="H22" r:id="rId14"/>
-    <hyperlink ref="H23" r:id="rId15"/>
-    <hyperlink ref="H24" r:id="rId16"/>
-    <hyperlink ref="H25" r:id="rId17"/>
-    <hyperlink ref="H26" r:id="rId18"/>
-    <hyperlink ref="H27" r:id="rId19"/>
-    <hyperlink ref="H29" r:id="rId20"/>
-    <hyperlink ref="H30" r:id="rId21"/>
-    <hyperlink ref="H31" r:id="rId22"/>
-    <hyperlink ref="H32" r:id="rId23"/>
-    <hyperlink ref="H33" r:id="rId24"/>
-    <hyperlink ref="H34" r:id="rId25"/>
-    <hyperlink ref="H35" r:id="rId26"/>
-    <hyperlink ref="H37" r:id="rId27"/>
-    <hyperlink ref="H38" r:id="rId28"/>
-    <hyperlink ref="H39" r:id="rId29"/>
-    <hyperlink ref="H40" r:id="rId30"/>
-    <hyperlink ref="H41" r:id="rId31"/>
-    <hyperlink ref="H42" r:id="rId32"/>
-    <hyperlink ref="H43" r:id="rId33"/>
-    <hyperlink ref="H44" r:id="rId34"/>
-    <hyperlink ref="H45" r:id="rId35"/>
-    <hyperlink ref="H46" r:id="rId36"/>
-    <hyperlink ref="F48" r:id="rId37"/>
-    <hyperlink ref="F49" r:id="rId38"/>
-    <hyperlink ref="F50" r:id="rId39"/>
-    <hyperlink ref="F51" r:id="rId40"/>
-    <hyperlink ref="F52" r:id="rId41"/>
-    <hyperlink ref="F53" r:id="rId42"/>
-    <hyperlink ref="F54" r:id="rId43"/>
-    <hyperlink ref="F55" r:id="rId44"/>
-    <hyperlink ref="F56" r:id="rId45"/>
-    <hyperlink ref="F57" r:id="rId46"/>
-    <hyperlink ref="F58" r:id="rId47"/>
-    <hyperlink ref="F59" r:id="rId48"/>
-    <hyperlink ref="F60" r:id="rId49"/>
-    <hyperlink ref="F61" r:id="rId50"/>
-    <hyperlink ref="F62" r:id="rId51"/>
-    <hyperlink ref="F63" r:id="rId52"/>
-    <hyperlink ref="F64" r:id="rId53"/>
-    <hyperlink ref="F65" r:id="rId54"/>
-    <hyperlink ref="F66" r:id="rId55"/>
-    <hyperlink ref="F67" r:id="rId56"/>
-    <hyperlink ref="F68" r:id="rId57"/>
-    <hyperlink ref="F69" r:id="rId58"/>
-    <hyperlink ref="F70" r:id="rId59"/>
-    <hyperlink ref="F71" r:id="rId60"/>
-    <hyperlink ref="F72" r:id="rId61"/>
-    <hyperlink ref="F73" r:id="rId62"/>
-    <hyperlink ref="F74" r:id="rId63"/>
-    <hyperlink ref="F75" r:id="rId64"/>
-    <hyperlink ref="F76" r:id="rId65"/>
-    <hyperlink ref="F77" r:id="rId66"/>
-    <hyperlink ref="F78" r:id="rId67"/>
-    <hyperlink ref="F79" r:id="rId68"/>
-    <hyperlink ref="F80" r:id="rId69"/>
-    <hyperlink ref="F81" r:id="rId70"/>
-    <hyperlink ref="F82" r:id="rId71"/>
-    <hyperlink ref="F83" r:id="rId72"/>
-    <hyperlink ref="F84" r:id="rId73"/>
-    <hyperlink ref="F85" r:id="rId74"/>
-    <hyperlink ref="F86" r:id="rId75"/>
-    <hyperlink ref="F87" r:id="rId76"/>
-    <hyperlink ref="F88" r:id="rId77"/>
+    <hyperlink ref="H16" r:id="rId8"/>
+    <hyperlink ref="H17" r:id="rId9"/>
+    <hyperlink ref="H18" r:id="rId10"/>
+    <hyperlink ref="H19" r:id="rId11"/>
+    <hyperlink ref="H20" r:id="rId12"/>
+    <hyperlink ref="H21" r:id="rId13"/>
+    <hyperlink ref="H23" r:id="rId14"/>
+    <hyperlink ref="H24" r:id="rId15"/>
+    <hyperlink ref="H25" r:id="rId16"/>
+    <hyperlink ref="H26" r:id="rId17"/>
+    <hyperlink ref="H27" r:id="rId18"/>
+    <hyperlink ref="H28" r:id="rId19"/>
+    <hyperlink ref="H30" r:id="rId20"/>
+    <hyperlink ref="H31" r:id="rId21"/>
+    <hyperlink ref="H32" r:id="rId22"/>
+    <hyperlink ref="H33" r:id="rId23"/>
+    <hyperlink ref="H34" r:id="rId24"/>
+    <hyperlink ref="H35" r:id="rId25"/>
+    <hyperlink ref="H36" r:id="rId26"/>
+    <hyperlink ref="H38" r:id="rId27"/>
+    <hyperlink ref="H39" r:id="rId28"/>
+    <hyperlink ref="H40" r:id="rId29"/>
+    <hyperlink ref="H41" r:id="rId30"/>
+    <hyperlink ref="H42" r:id="rId31"/>
+    <hyperlink ref="H43" r:id="rId32"/>
+    <hyperlink ref="H44" r:id="rId33"/>
+    <hyperlink ref="H45" r:id="rId34"/>
+    <hyperlink ref="H46" r:id="rId35"/>
+    <hyperlink ref="H47" r:id="rId36"/>
+    <hyperlink ref="F49" r:id="rId37"/>
+    <hyperlink ref="F50" r:id="rId38"/>
+    <hyperlink ref="F51" r:id="rId39"/>
+    <hyperlink ref="F52" r:id="rId40"/>
+    <hyperlink ref="F53" r:id="rId41"/>
+    <hyperlink ref="F54" r:id="rId42"/>
+    <hyperlink ref="F55" r:id="rId43"/>
+    <hyperlink ref="F56" r:id="rId44"/>
+    <hyperlink ref="F57" r:id="rId45"/>
+    <hyperlink ref="F58" r:id="rId46"/>
+    <hyperlink ref="F59" r:id="rId47"/>
+    <hyperlink ref="F60" r:id="rId48"/>
+    <hyperlink ref="F61" r:id="rId49"/>
+    <hyperlink ref="F62" r:id="rId50"/>
+    <hyperlink ref="F63" r:id="rId51"/>
+    <hyperlink ref="F64" r:id="rId52"/>
+    <hyperlink ref="F65" r:id="rId53"/>
+    <hyperlink ref="F66" r:id="rId54"/>
+    <hyperlink ref="F67" r:id="rId55"/>
+    <hyperlink ref="F68" r:id="rId56"/>
+    <hyperlink ref="F69" r:id="rId57"/>
+    <hyperlink ref="F70" r:id="rId58"/>
+    <hyperlink ref="F71" r:id="rId59"/>
+    <hyperlink ref="F72" r:id="rId60"/>
+    <hyperlink ref="F73" r:id="rId61"/>
+    <hyperlink ref="F74" r:id="rId62"/>
+    <hyperlink ref="F75" r:id="rId63"/>
+    <hyperlink ref="F76" r:id="rId64"/>
+    <hyperlink ref="F77" r:id="rId65"/>
+    <hyperlink ref="F78" r:id="rId66"/>
+    <hyperlink ref="F79" r:id="rId67"/>
+    <hyperlink ref="F80" r:id="rId68"/>
+    <hyperlink ref="F81" r:id="rId69"/>
+    <hyperlink ref="F82" r:id="rId70"/>
+    <hyperlink ref="F83" r:id="rId71"/>
+    <hyperlink ref="F84" r:id="rId72"/>
+    <hyperlink ref="F85" r:id="rId73"/>
+    <hyperlink ref="F86" r:id="rId74"/>
+    <hyperlink ref="F87" r:id="rId75"/>
+    <hyperlink ref="F88" r:id="rId76"/>
+    <hyperlink ref="F89" r:id="rId77"/>
     <hyperlink ref="H5" r:id="rId78"/>
     <hyperlink ref="H7" r:id="rId79"/>
     <hyperlink ref="H6" r:id="rId80"/>
@@ -4213,15 +4248,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="52" t="s">
         <v>316</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="13" t="s">

</xml_diff>